<commit_message>
All Pennik models working.
</commit_message>
<xml_diff>
--- a/Projects/Pennink-Model/cases/Boogkanaal1/Boogkanaal1.xlsx
+++ b/Projects/Pennink-Model/cases/Boogkanaal1/Boogkanaal1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/GRWMODELS/python/mf6lab/Projects/Pennink-Model/cases/Boogkanaal1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F13443-8AB7-D241-A5BD-8F3FDDF0E35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0800BF6-848D-F142-ADFA-1EC8F097FE92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9820" yWindow="-24220" windowWidth="28180" windowHeight="16980" tabRatio="751" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3640" yWindow="2280" windowWidth="28180" windowHeight="16980" tabRatio="751" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NAM" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2458" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2456" uniqueCount="424">
   <si>
     <t>ON / OFF</t>
   </si>
@@ -1397,7 +1397,7 @@
     <t>Days</t>
   </si>
   <si>
-    <t>COMPLEX</t>
+    <t>NEWTON</t>
   </si>
 </sst>
 </file>
@@ -2627,7 +2627,7 @@
   <dimension ref="A1:C115"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3492,8 +3492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C06500DB-BECE-8C4B-B4E6-A47BC546FCEB}">
   <dimension ref="A1:H477"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3618,7 +3618,7 @@
         <v>108</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>423</v>
+        <v>379</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>380</v>
@@ -3697,8 +3697,8 @@
       <c r="B18" t="s">
         <v>115</v>
       </c>
-      <c r="C18" t="s">
-        <v>19</v>
+      <c r="C18">
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
@@ -3719,8 +3719,8 @@
       <c r="B20" t="s">
         <v>117</v>
       </c>
-      <c r="C20" t="s">
-        <v>19</v>
+      <c r="C20">
+        <v>800</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
@@ -5777,7 +5777,7 @@
         <v>43</v>
       </c>
       <c r="C218" s="9" t="s">
-        <v>382</v>
+        <v>423</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.15">
@@ -11786,7 +11786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="264" zoomScaleNormal="264" workbookViewId="0">
+    <sheetView zoomScale="264" zoomScaleNormal="264" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>